<commit_message>
update file for assignment 9
</commit_message>
<xml_diff>
--- a/unit9-integer optimization/PfizerReps.xlsx
+++ b/unit9-integer optimization/PfizerReps.xlsx
@@ -1,15 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="1340" windowWidth="17580" windowHeight="14680" tabRatio="500"/>
+    <workbookView xWindow="795" yWindow="1335" windowWidth="17580" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$B$66:$E$87</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_lhs0" localSheetId="0" hidden="1">Sheet1!$B$88:$E$88</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$B$66:$E$87</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$B$89:$E$89</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$B$88:$E$88</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Sheet1!$B$88:$E$88</definedName>
+    <definedName name="solver_lhs5" localSheetId="0" hidden="1">Sheet1!$F$66:$F$87</definedName>
+    <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">5</definedName>
+    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$B$91</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rel0" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="0" hidden="1">5</definedName>
+    <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rhs0" localSheetId="0" hidden="1">0.8</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">二进制</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">0.7</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">1.2</definedName>
+    <definedName name="solver_rhs5" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">200</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.05</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+  </definedNames>
+  <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>ASSIGNING SALES REGIONS AT PFIZER TURKEY</t>
   </si>
@@ -85,17 +122,216 @@
   </si>
   <si>
     <t>Distance to Office of SR 4</t>
+  </si>
+  <si>
+    <t>decision variables</t>
+  </si>
+  <si>
+    <t>objective</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>each brick must be assigned to exactly one SR</t>
+  </si>
+  <si>
+    <t>constraints</t>
+  </si>
+  <si>
+    <t>LHS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sign</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RHS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>=</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">sum(X_1~4, j) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum(X_1~4, j) </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>workload</t>
+  </si>
+  <si>
+    <t>[0.8, 1.2]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>between</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">workload </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>workload</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>disruption</t>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8.4499999999999993"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.4499999999999993"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Main"/>
+        <family val="2"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8.4499999999999993"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+        <family val="2"/>
+      </rPr>
+      <t>j</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, where </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14.85"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+        <family val="2"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8.4499999999999993"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.4499999999999993"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Main"/>
+        <family val="2"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8.4499999999999993"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+        <family val="2"/>
+      </rPr>
+      <t>j</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is equal to 1 if brick </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14.85"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+        <family val="2"/>
+      </rPr>
+      <t>j</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is assigned to SR </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14.85"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <t>disruption</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;=</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -103,20 +339,68 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8.4499999999999993"/>
+      <color theme="1"/>
+      <name val="MathJax_Math"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14.85"/>
+      <color theme="1"/>
+      <name val="MathJax_Math"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8.4499999999999993"/>
+      <color theme="1"/>
+      <name val="MathJax_Main"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -210,11 +494,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -280,12 +638,90 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FF00"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -610,23 +1046,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66:E87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" customWidth="1"/>
-    <col min="3" max="3" width="27.1640625" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.875" customWidth="1"/>
+    <col min="2" max="2" width="22.125" customWidth="1"/>
+    <col min="3" max="3" width="27.125" customWidth="1"/>
+    <col min="4" max="4" width="23.375" customWidth="1"/>
+    <col min="5" max="5" width="22.375" customWidth="1"/>
+    <col min="9" max="9" width="16.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -638,7 +1075,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
@@ -648,7 +1085,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="2"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
@@ -658,7 +1095,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" s="22" customFormat="1" ht="16" thickBot="1">
+    <row r="4" spans="1:9" s="22" customFormat="1" ht="15" thickBot="1">
       <c r="A4" s="19" t="s">
         <v>1</v>
       </c>
@@ -672,7 +1109,7 @@
       <c r="G4" s="21"/>
       <c r="H4" s="21"/>
     </row>
-    <row r="5" spans="1:8" ht="16" thickBot="1">
+    <row r="5" spans="1:9" ht="29.25" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -685,20 +1122,21 @@
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="26" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" s="28"/>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="7">
         <v>1</v>
       </c>
@@ -711,20 +1149,21 @@
       <c r="D6" s="7">
         <v>1</v>
       </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="9">
-        <v>1</v>
-      </c>
-      <c r="G6" s="9">
-        <v>1</v>
-      </c>
-      <c r="H6" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="E6" s="40">
+        <v>1</v>
+      </c>
+      <c r="F6" s="41">
+        <v>1</v>
+      </c>
+      <c r="G6" s="41">
+        <v>1</v>
+      </c>
+      <c r="H6" s="41">
+        <v>0</v>
+      </c>
+      <c r="I6" s="44"/>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="7">
         <v>2</v>
       </c>
@@ -737,20 +1176,21 @@
       <c r="D7" s="7">
         <v>2</v>
       </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="9">
-        <v>1</v>
-      </c>
-      <c r="G7" s="9">
-        <v>1</v>
-      </c>
-      <c r="H7" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="E7" s="40">
+        <v>1</v>
+      </c>
+      <c r="F7" s="41">
+        <v>1</v>
+      </c>
+      <c r="G7" s="41">
+        <v>1</v>
+      </c>
+      <c r="H7" s="41">
+        <v>0</v>
+      </c>
+      <c r="I7" s="44"/>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="7">
         <v>3</v>
       </c>
@@ -763,20 +1203,21 @@
       <c r="D8" s="7">
         <v>3</v>
       </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="9">
-        <v>1</v>
-      </c>
-      <c r="G8" s="9">
-        <v>1</v>
-      </c>
-      <c r="H8" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="16" thickBot="1">
+      <c r="E8" s="40">
+        <v>1</v>
+      </c>
+      <c r="F8" s="41">
+        <v>1</v>
+      </c>
+      <c r="G8" s="41">
+        <v>1</v>
+      </c>
+      <c r="H8" s="41">
+        <v>0</v>
+      </c>
+      <c r="I8" s="44"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" thickBot="1">
       <c r="A9" s="11">
         <v>4</v>
       </c>
@@ -789,60 +1230,63 @@
       <c r="D9" s="7">
         <v>4</v>
       </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="9">
-        <v>1</v>
-      </c>
-      <c r="G9" s="9">
-        <v>1</v>
-      </c>
-      <c r="H9" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="E9" s="40">
+        <v>0</v>
+      </c>
+      <c r="F9" s="41">
+        <v>1</v>
+      </c>
+      <c r="G9" s="41">
+        <v>1</v>
+      </c>
+      <c r="H9" s="41">
+        <v>1</v>
+      </c>
+      <c r="I9" s="44"/>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
       <c r="D10" s="7">
         <v>5</v>
       </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="9">
-        <v>1</v>
-      </c>
-      <c r="G10" s="9">
-        <v>1</v>
-      </c>
-      <c r="H10" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="E10" s="40">
+        <v>0</v>
+      </c>
+      <c r="F10" s="41">
+        <v>1</v>
+      </c>
+      <c r="G10" s="41">
+        <v>1</v>
+      </c>
+      <c r="H10" s="41">
+        <v>1</v>
+      </c>
+      <c r="I10" s="44"/>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="2"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
       <c r="D11" s="7">
         <v>6</v>
       </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="9">
-        <v>1</v>
-      </c>
-      <c r="G11" s="9">
-        <v>1</v>
-      </c>
-      <c r="H11" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="16" thickBot="1">
+      <c r="E11" s="40">
+        <v>0</v>
+      </c>
+      <c r="F11" s="41">
+        <v>1</v>
+      </c>
+      <c r="G11" s="41">
+        <v>1</v>
+      </c>
+      <c r="H11" s="41">
+        <v>1</v>
+      </c>
+      <c r="I11" s="44"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" thickBot="1">
       <c r="A12" s="19" t="s">
         <v>15</v>
       </c>
@@ -851,20 +1295,21 @@
       <c r="D12" s="7">
         <v>7</v>
       </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-      <c r="F12" s="9">
-        <v>1</v>
-      </c>
-      <c r="G12" s="9">
-        <v>1</v>
-      </c>
-      <c r="H12" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="16" thickBot="1">
+      <c r="E12" s="40">
+        <v>0</v>
+      </c>
+      <c r="F12" s="41">
+        <v>1</v>
+      </c>
+      <c r="G12" s="41">
+        <v>1</v>
+      </c>
+      <c r="H12" s="41">
+        <v>1</v>
+      </c>
+      <c r="I12" s="44"/>
+    </row>
+    <row r="13" spans="1:9" ht="29.25" thickBot="1">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -875,20 +1320,21 @@
       <c r="D13" s="7">
         <v>8</v>
       </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-      <c r="F13" s="9">
-        <v>1</v>
-      </c>
-      <c r="G13" s="9">
-        <v>1</v>
-      </c>
-      <c r="H13" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="E13" s="40">
+        <v>0</v>
+      </c>
+      <c r="F13" s="41">
+        <v>1</v>
+      </c>
+      <c r="G13" s="41">
+        <v>1</v>
+      </c>
+      <c r="H13" s="41">
+        <v>1</v>
+      </c>
+      <c r="I13" s="44"/>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="7">
         <v>1</v>
       </c>
@@ -899,20 +1345,21 @@
       <c r="D14" s="7">
         <v>9</v>
       </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-      <c r="F14" s="9">
-        <v>1</v>
-      </c>
-      <c r="G14" s="9">
-        <v>0</v>
-      </c>
-      <c r="H14" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="E14" s="40">
+        <v>1</v>
+      </c>
+      <c r="F14" s="41">
+        <v>1</v>
+      </c>
+      <c r="G14" s="41">
+        <v>0</v>
+      </c>
+      <c r="H14" s="41">
+        <v>1</v>
+      </c>
+      <c r="I14" s="44"/>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="7">
         <v>2</v>
       </c>
@@ -923,20 +1370,21 @@
       <c r="D15" s="7">
         <v>10</v>
       </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-      <c r="F15" s="9">
-        <v>0</v>
-      </c>
-      <c r="G15" s="9">
-        <v>1</v>
-      </c>
-      <c r="H15" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="E15" s="40">
+        <v>1</v>
+      </c>
+      <c r="F15" s="41">
+        <v>0</v>
+      </c>
+      <c r="G15" s="41">
+        <v>1</v>
+      </c>
+      <c r="H15" s="41">
+        <v>1</v>
+      </c>
+      <c r="I15" s="44"/>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="7">
         <v>3</v>
       </c>
@@ -947,20 +1395,21 @@
       <c r="D16" s="7">
         <v>11</v>
       </c>
-      <c r="E16" s="1">
-        <v>1</v>
-      </c>
-      <c r="F16" s="9">
-        <v>0</v>
-      </c>
-      <c r="G16" s="9">
-        <v>1</v>
-      </c>
-      <c r="H16" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="E16" s="40">
+        <v>1</v>
+      </c>
+      <c r="F16" s="41">
+        <v>0</v>
+      </c>
+      <c r="G16" s="41">
+        <v>1</v>
+      </c>
+      <c r="H16" s="41">
+        <v>1</v>
+      </c>
+      <c r="I16" s="44"/>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="7">
         <v>4</v>
       </c>
@@ -971,20 +1420,21 @@
       <c r="D17" s="7">
         <v>12</v>
       </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="F17" s="9">
-        <v>0</v>
-      </c>
-      <c r="G17" s="9">
-        <v>1</v>
-      </c>
-      <c r="H17" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="E17" s="40">
+        <v>1</v>
+      </c>
+      <c r="F17" s="41">
+        <v>0</v>
+      </c>
+      <c r="G17" s="41">
+        <v>1</v>
+      </c>
+      <c r="H17" s="41">
+        <v>1</v>
+      </c>
+      <c r="I17" s="44"/>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="7">
         <v>5</v>
       </c>
@@ -995,20 +1445,21 @@
       <c r="D18" s="7">
         <v>13</v>
       </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
-      <c r="F18" s="9">
-        <v>0</v>
-      </c>
-      <c r="G18" s="9">
-        <v>1</v>
-      </c>
-      <c r="H18" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="E18" s="40">
+        <v>1</v>
+      </c>
+      <c r="F18" s="41">
+        <v>0</v>
+      </c>
+      <c r="G18" s="41">
+        <v>1</v>
+      </c>
+      <c r="H18" s="41">
+        <v>1</v>
+      </c>
+      <c r="I18" s="44"/>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="7">
         <v>6</v>
       </c>
@@ -1019,20 +1470,21 @@
       <c r="D19" s="7">
         <v>14</v>
       </c>
-      <c r="E19" s="1">
-        <v>1</v>
-      </c>
-      <c r="F19" s="9">
-        <v>0</v>
-      </c>
-      <c r="G19" s="9">
-        <v>1</v>
-      </c>
-      <c r="H19" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="E19" s="40">
+        <v>1</v>
+      </c>
+      <c r="F19" s="41">
+        <v>0</v>
+      </c>
+      <c r="G19" s="41">
+        <v>1</v>
+      </c>
+      <c r="H19" s="41">
+        <v>1</v>
+      </c>
+      <c r="I19" s="44"/>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="7">
         <v>7</v>
       </c>
@@ -1043,20 +1495,21 @@
       <c r="D20" s="7">
         <v>15</v>
       </c>
-      <c r="E20" s="1">
-        <v>0</v>
-      </c>
-      <c r="F20" s="9">
-        <v>1</v>
-      </c>
-      <c r="G20" s="9">
-        <v>1</v>
-      </c>
-      <c r="H20" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="E20" s="40">
+        <v>0</v>
+      </c>
+      <c r="F20" s="41">
+        <v>1</v>
+      </c>
+      <c r="G20" s="41">
+        <v>1</v>
+      </c>
+      <c r="H20" s="41">
+        <v>1</v>
+      </c>
+      <c r="I20" s="44"/>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="7">
         <v>8</v>
       </c>
@@ -1067,20 +1520,21 @@
       <c r="D21" s="7">
         <v>16</v>
       </c>
-      <c r="E21" s="1">
-        <v>1</v>
-      </c>
-      <c r="F21" s="9">
-        <v>1</v>
-      </c>
-      <c r="G21" s="9">
-        <v>0</v>
-      </c>
-      <c r="H21" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="E21" s="40">
+        <v>1</v>
+      </c>
+      <c r="F21" s="41">
+        <v>1</v>
+      </c>
+      <c r="G21" s="41">
+        <v>0</v>
+      </c>
+      <c r="H21" s="41">
+        <v>1</v>
+      </c>
+      <c r="I21" s="44"/>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="7">
         <v>9</v>
       </c>
@@ -1091,20 +1545,21 @@
       <c r="D22" s="7">
         <v>17</v>
       </c>
-      <c r="E22" s="1">
-        <v>1</v>
-      </c>
-      <c r="F22" s="9">
-        <v>1</v>
-      </c>
-      <c r="G22" s="9">
-        <v>0</v>
-      </c>
-      <c r="H22" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="E22" s="40">
+        <v>1</v>
+      </c>
+      <c r="F22" s="41">
+        <v>1</v>
+      </c>
+      <c r="G22" s="41">
+        <v>0</v>
+      </c>
+      <c r="H22" s="41">
+        <v>1</v>
+      </c>
+      <c r="I22" s="44"/>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="7">
         <v>10</v>
       </c>
@@ -1115,20 +1570,21 @@
       <c r="D23" s="7">
         <v>18</v>
       </c>
-      <c r="E23" s="1">
-        <v>1</v>
-      </c>
-      <c r="F23" s="9">
-        <v>1</v>
-      </c>
-      <c r="G23" s="9">
-        <v>0</v>
-      </c>
-      <c r="H23" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="E23" s="40">
+        <v>1</v>
+      </c>
+      <c r="F23" s="41">
+        <v>1</v>
+      </c>
+      <c r="G23" s="41">
+        <v>0</v>
+      </c>
+      <c r="H23" s="41">
+        <v>1</v>
+      </c>
+      <c r="I23" s="44"/>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="7">
         <v>11</v>
       </c>
@@ -1139,20 +1595,21 @@
       <c r="D24" s="7">
         <v>19</v>
       </c>
-      <c r="E24" s="1">
-        <v>1</v>
-      </c>
-      <c r="F24" s="9">
-        <v>1</v>
-      </c>
-      <c r="G24" s="9">
-        <v>1</v>
-      </c>
-      <c r="H24" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="E24" s="40">
+        <v>1</v>
+      </c>
+      <c r="F24" s="41">
+        <v>1</v>
+      </c>
+      <c r="G24" s="41">
+        <v>1</v>
+      </c>
+      <c r="H24" s="41">
+        <v>0</v>
+      </c>
+      <c r="I24" s="44"/>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="7">
         <v>12</v>
       </c>
@@ -1163,20 +1620,21 @@
       <c r="D25" s="7">
         <v>20</v>
       </c>
-      <c r="E25" s="1">
-        <v>1</v>
-      </c>
-      <c r="F25" s="9">
-        <v>1</v>
-      </c>
-      <c r="G25" s="9">
-        <v>1</v>
-      </c>
-      <c r="H25" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="E25" s="40">
+        <v>1</v>
+      </c>
+      <c r="F25" s="41">
+        <v>1</v>
+      </c>
+      <c r="G25" s="41">
+        <v>1</v>
+      </c>
+      <c r="H25" s="41">
+        <v>0</v>
+      </c>
+      <c r="I25" s="44"/>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="7">
         <v>13</v>
       </c>
@@ -1187,20 +1645,21 @@
       <c r="D26" s="7">
         <v>21</v>
       </c>
-      <c r="E26" s="1">
-        <v>1</v>
-      </c>
-      <c r="F26" s="9">
-        <v>1</v>
-      </c>
-      <c r="G26" s="9">
-        <v>1</v>
-      </c>
-      <c r="H26" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="16" thickBot="1">
+      <c r="E26" s="42">
+        <v>1</v>
+      </c>
+      <c r="F26" s="43">
+        <v>1</v>
+      </c>
+      <c r="G26" s="43">
+        <v>1</v>
+      </c>
+      <c r="H26" s="43">
+        <v>0</v>
+      </c>
+      <c r="I26" s="44"/>
+    </row>
+    <row r="27" spans="1:9" ht="15" thickBot="1">
       <c r="A27" s="7">
         <v>14</v>
       </c>
@@ -1208,23 +1667,24 @@
         <v>0.81769999999999998</v>
       </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="11">
+      <c r="D27" s="49">
         <v>22</v>
       </c>
-      <c r="E27" s="12">
-        <v>1</v>
-      </c>
-      <c r="F27" s="16">
-        <v>1</v>
-      </c>
-      <c r="G27" s="16">
-        <v>1</v>
-      </c>
-      <c r="H27" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="E27" s="47">
+        <v>1</v>
+      </c>
+      <c r="F27" s="48">
+        <v>1</v>
+      </c>
+      <c r="G27" s="48">
+        <v>1</v>
+      </c>
+      <c r="H27" s="48">
+        <v>0</v>
+      </c>
+      <c r="I27" s="44"/>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="7">
         <v>15</v>
       </c>
@@ -1232,13 +1692,13 @@
         <v>0.41149999999999998</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="D28" s="45"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="7">
         <v>16</v>
       </c>
@@ -1252,7 +1712,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:9">
       <c r="A30" s="7">
         <v>17</v>
       </c>
@@ -1266,7 +1726,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:9">
       <c r="A31" s="7">
         <v>18</v>
       </c>
@@ -1280,7 +1740,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:9">
       <c r="A32" s="7">
         <v>19</v>
       </c>
@@ -1322,7 +1782,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" ht="16" thickBot="1">
+    <row r="35" spans="1:8" ht="15" thickBot="1">
       <c r="A35" s="11">
         <v>22</v>
       </c>
@@ -1356,7 +1816,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" ht="16" thickBot="1">
+    <row r="38" spans="1:8" ht="15" thickBot="1">
       <c r="A38" s="19" t="s">
         <v>17</v>
       </c>
@@ -1368,7 +1828,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" ht="16" thickBot="1">
+    <row r="39" spans="1:8" ht="29.25" thickBot="1">
       <c r="A39" s="3" t="s">
         <v>6</v>
       </c>
@@ -1808,7 +2268,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" ht="16" thickBot="1">
+    <row r="61" spans="1:8" ht="15" thickBot="1">
       <c r="A61" s="11">
         <v>22</v>
       </c>
@@ -1828,7 +2288,680 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="34"/>
+      <c r="B62" s="35"/>
+      <c r="C62" s="35"/>
+      <c r="D62" s="35"/>
+      <c r="E62" s="35"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+    </row>
+    <row r="63" spans="1:8" ht="19.5">
+      <c r="A63" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B63" s="35"/>
+      <c r="C63" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D63" s="35"/>
+      <c r="E63" s="35"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="34"/>
+      <c r="B64" s="35"/>
+      <c r="C64" s="35"/>
+      <c r="D64" s="35"/>
+      <c r="E64" s="35"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+    </row>
+    <row r="65" spans="1:8" ht="28.5">
+      <c r="A65" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F65" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="38">
+        <v>1</v>
+      </c>
+      <c r="B66" s="27">
+        <v>0</v>
+      </c>
+      <c r="C66" s="27">
+        <v>0</v>
+      </c>
+      <c r="D66" s="27">
+        <v>0</v>
+      </c>
+      <c r="E66" s="27">
+        <v>1</v>
+      </c>
+      <c r="F66" s="29">
+        <f>SUM(B66:E66)</f>
+        <v>1</v>
+      </c>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="38">
+        <v>2</v>
+      </c>
+      <c r="B67" s="27">
+        <v>0</v>
+      </c>
+      <c r="C67" s="27">
+        <v>0</v>
+      </c>
+      <c r="D67" s="27">
+        <v>0</v>
+      </c>
+      <c r="E67" s="27">
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="F67" s="29">
+        <f t="shared" ref="F67:F87" si="0">SUM(B67:E67)</f>
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="38">
+        <v>3</v>
+      </c>
+      <c r="B68" s="27">
+        <v>0</v>
+      </c>
+      <c r="C68" s="27">
+        <v>0</v>
+      </c>
+      <c r="D68" s="27">
+        <v>0</v>
+      </c>
+      <c r="E68" s="27">
+        <v>1</v>
+      </c>
+      <c r="F68" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="38">
+        <v>4</v>
+      </c>
+      <c r="B69" s="27">
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="C69" s="27">
+        <v>0</v>
+      </c>
+      <c r="D69" s="27">
+        <v>0</v>
+      </c>
+      <c r="E69" s="27">
+        <v>0</v>
+      </c>
+      <c r="F69" s="29">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="38">
+        <v>5</v>
+      </c>
+      <c r="B70" s="27">
+        <v>1</v>
+      </c>
+      <c r="C70" s="27">
+        <v>0</v>
+      </c>
+      <c r="D70" s="27">
+        <v>0</v>
+      </c>
+      <c r="E70" s="27">
+        <v>0</v>
+      </c>
+      <c r="F70" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="38">
+        <v>6</v>
+      </c>
+      <c r="B71" s="27">
+        <v>1</v>
+      </c>
+      <c r="C71" s="27">
+        <v>0</v>
+      </c>
+      <c r="D71" s="27">
+        <v>0</v>
+      </c>
+      <c r="E71" s="27">
+        <v>0</v>
+      </c>
+      <c r="F71" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="38">
+        <v>7</v>
+      </c>
+      <c r="B72" s="27">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="C72" s="27">
+        <v>0</v>
+      </c>
+      <c r="D72" s="27">
+        <v>0</v>
+      </c>
+      <c r="E72" s="27">
+        <v>0</v>
+      </c>
+      <c r="F72" s="29">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="38">
+        <v>8</v>
+      </c>
+      <c r="B73" s="27">
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="C73" s="27">
+        <v>0</v>
+      </c>
+      <c r="D73" s="27">
+        <v>0</v>
+      </c>
+      <c r="E73" s="27">
+        <v>0</v>
+      </c>
+      <c r="F73" s="29">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="38">
+        <v>9</v>
+      </c>
+      <c r="B74" s="27">
+        <v>0.99999999999999956</v>
+      </c>
+      <c r="C74" s="27">
+        <v>0</v>
+      </c>
+      <c r="D74" s="27">
+        <v>0</v>
+      </c>
+      <c r="E74" s="27">
+        <v>0</v>
+      </c>
+      <c r="F74" s="29">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999956</v>
+      </c>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="38">
+        <v>10</v>
+      </c>
+      <c r="B75" s="27">
+        <v>1.1049199594705031E-16</v>
+      </c>
+      <c r="C75" s="27">
+        <v>0</v>
+      </c>
+      <c r="D75" s="27">
+        <v>1</v>
+      </c>
+      <c r="E75" s="27">
+        <v>0</v>
+      </c>
+      <c r="F75" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="38">
+        <v>11</v>
+      </c>
+      <c r="B76" s="27">
+        <v>6.7132324005348229E-17</v>
+      </c>
+      <c r="C76" s="27">
+        <v>1</v>
+      </c>
+      <c r="D76" s="27">
+        <v>0</v>
+      </c>
+      <c r="E76" s="27">
+        <v>0</v>
+      </c>
+      <c r="F76" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="38">
+        <v>12</v>
+      </c>
+      <c r="B77" s="27">
+        <v>9.7766575651164755E-16</v>
+      </c>
+      <c r="C77" s="27">
+        <v>0.999999999999999</v>
+      </c>
+      <c r="D77" s="27">
+        <v>0</v>
+      </c>
+      <c r="E77" s="27">
+        <v>0</v>
+      </c>
+      <c r="F77" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" s="38">
+        <v>13</v>
+      </c>
+      <c r="B78" s="27">
+        <v>0</v>
+      </c>
+      <c r="C78" s="27">
+        <v>1</v>
+      </c>
+      <c r="D78" s="27">
+        <v>0</v>
+      </c>
+      <c r="E78" s="27">
+        <v>0</v>
+      </c>
+      <c r="F78" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" s="38">
+        <v>14</v>
+      </c>
+      <c r="B79" s="27">
+        <v>0</v>
+      </c>
+      <c r="C79" s="27">
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="D79" s="27">
+        <v>0</v>
+      </c>
+      <c r="E79" s="27">
+        <v>0</v>
+      </c>
+      <c r="F79" s="29">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="G79" s="2"/>
+      <c r="H79" s="2"/>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="38">
+        <v>15</v>
+      </c>
+      <c r="B80" s="27">
+        <v>0</v>
+      </c>
+      <c r="C80" s="27">
+        <v>0</v>
+      </c>
+      <c r="D80" s="27">
+        <v>1</v>
+      </c>
+      <c r="E80" s="27">
+        <v>0</v>
+      </c>
+      <c r="F80" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" s="38">
+        <v>16</v>
+      </c>
+      <c r="B81" s="27">
+        <v>0</v>
+      </c>
+      <c r="C81" s="27">
+        <v>-9.8069120912144082E-17</v>
+      </c>
+      <c r="D81" s="27">
+        <v>1</v>
+      </c>
+      <c r="E81" s="27">
+        <v>0</v>
+      </c>
+      <c r="F81" s="29">
+        <f>SUM(B81:E81)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" s="38">
+        <v>17</v>
+      </c>
+      <c r="B82" s="27">
+        <v>0</v>
+      </c>
+      <c r="C82" s="27">
+        <v>0</v>
+      </c>
+      <c r="D82" s="27">
+        <v>1</v>
+      </c>
+      <c r="E82" s="27">
+        <v>0</v>
+      </c>
+      <c r="F82" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" s="38">
+        <v>18</v>
+      </c>
+      <c r="B83" s="27">
+        <v>1.4528378500244806E-16</v>
+      </c>
+      <c r="C83" s="27">
+        <v>0</v>
+      </c>
+      <c r="D83" s="27">
+        <v>1</v>
+      </c>
+      <c r="E83" s="27">
+        <v>0</v>
+      </c>
+      <c r="F83" s="29">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2"/>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" s="38">
+        <v>19</v>
+      </c>
+      <c r="B84" s="27">
+        <v>0</v>
+      </c>
+      <c r="C84" s="27">
+        <v>1</v>
+      </c>
+      <c r="D84" s="27">
+        <v>0</v>
+      </c>
+      <c r="E84" s="27">
+        <v>0</v>
+      </c>
+      <c r="F84" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G84" s="2"/>
+      <c r="H84" s="2"/>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85" s="38">
+        <v>20</v>
+      </c>
+      <c r="B85" s="27">
+        <v>0</v>
+      </c>
+      <c r="C85" s="27">
+        <v>0</v>
+      </c>
+      <c r="D85" s="27">
+        <v>0</v>
+      </c>
+      <c r="E85" s="27">
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="F85" s="29">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="G85" s="2"/>
+      <c r="H85" s="2"/>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="38">
+        <v>21</v>
+      </c>
+      <c r="B86" s="27">
+        <v>0.99999999999999878</v>
+      </c>
+      <c r="C86" s="27">
+        <v>0</v>
+      </c>
+      <c r="D86" s="27">
+        <v>0</v>
+      </c>
+      <c r="E86" s="27">
+        <v>0</v>
+      </c>
+      <c r="F86" s="29">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999878</v>
+      </c>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2"/>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" s="38">
+        <v>22</v>
+      </c>
+      <c r="B87" s="39">
+        <v>1.9914538768039985E-17</v>
+      </c>
+      <c r="C87" s="39">
+        <v>0</v>
+      </c>
+      <c r="D87" s="39">
+        <v>0</v>
+      </c>
+      <c r="E87" s="39">
+        <v>1</v>
+      </c>
+      <c r="F87" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B88" s="33">
+        <f>SUMPRODUCT(B66:B87,$B$14:$B$35)</f>
+        <v>0.92059999999999986</v>
+      </c>
+      <c r="C88" s="33">
+        <f t="shared" ref="C88:E88" si="1">SUMPRODUCT(C66:C87,$B$14:$B$35)</f>
+        <v>1.1890999999999998</v>
+      </c>
+      <c r="D88" s="33">
+        <f t="shared" si="1"/>
+        <v>1.1576</v>
+      </c>
+      <c r="E88" s="33">
+        <f t="shared" si="1"/>
+        <v>0.73270000000000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B89" s="33">
+        <f>SUMPRODUCT(B66:B87,E6:E27)</f>
+        <v>1.9999999999999996</v>
+      </c>
+      <c r="C89" s="33">
+        <f t="shared" ref="C89:E89" si="2">SUMPRODUCT(C66:C87,F6:F27)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="D89" s="33">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E89" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B91">
+        <f>SUMPRODUCT(B66:E87,B40:E61)</f>
+        <v>154.00999999999996</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="A92" s="23"/>
+    </row>
+    <row r="93" spans="1:8">
+      <c r="A93" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="B94" t="s">
+        <v>26</v>
+      </c>
+      <c r="C94" t="s">
+        <v>27</v>
+      </c>
+      <c r="D94" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="71.25">
+      <c r="A95" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B95" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C95" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D95" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
+      <c r="A96" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B96" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C96" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D96" s="51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B97" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C97" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="D97" s="51">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>